<commit_message>
cable fix 'n' trix
</commit_message>
<xml_diff>
--- a/data/T085 Hallonvagen.xlsx
+++ b/data/T085 Hallonvagen.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\GitHub\MasterThesisCode\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Exjobb\Matlab\MasterThesisCode\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D8F689-6ED4-4F68-A320-50836C598E44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="4980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4980"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -69,15 +68,9 @@
     <t>4   T085-0.4-S1</t>
   </si>
   <si>
-    <t>AKKJ240</t>
-  </si>
-  <si>
     <t>6   1159</t>
   </si>
   <si>
-    <t>EKKJ10</t>
-  </si>
-  <si>
     <t>8   233238</t>
   </si>
   <si>
@@ -253,12 +246,18 @@
   </si>
   <si>
     <t>N1XV4G10</t>
+  </si>
+  <si>
+    <t>AKKJ240/72</t>
+  </si>
+  <si>
+    <t>EKKJ10/10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -571,21 +570,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -623,7 +626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>90</v>
       </c>
@@ -658,7 +661,7 @@
         <v>1.7152192100000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>90</v>
       </c>
@@ -696,12 +699,12 @@
         <v>1.7154601799999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -734,18 +737,18 @@
         <v>0.13496383170000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>31</v>
@@ -772,15 +775,15 @@
         <v>0.15015742309999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -810,18 +813,18 @@
         <v>0.1540962736</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>31</v>
@@ -848,15 +851,15 @@
         <v>0.28089565579999998</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -886,18 +889,18 @@
         <v>0.15804592719999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11">
         <v>45</v>
@@ -924,15 +927,15 @@
         <v>0.3430087389</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -962,18 +965,18 @@
         <v>0.15804592719999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E13">
         <v>27</v>
@@ -1000,12 +1003,12 @@
         <v>0.26844479929999998</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -1038,18 +1041,18 @@
         <v>0.15800320700000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <v>59</v>
@@ -1076,18 +1079,18 @@
         <v>0.18695126249999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1114,18 +1117,18 @@
         <v>0.2642397655</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
         <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
       </c>
       <c r="E17">
         <v>45</v>
@@ -1152,15 +1155,15 @@
         <v>0.37156091270000002</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1190,18 +1193,18 @@
         <v>0.21880971739999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E19">
         <v>15</v>
@@ -1228,15 +1231,15 @@
         <v>0.28022384220000002</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>19</v>
@@ -1266,18 +1269,18 @@
         <v>0.33238627389999997</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E21">
         <v>9</v>
@@ -1304,15 +1307,15 @@
         <v>0.36969992740000002</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>21</v>
@@ -1342,18 +1345,18 @@
         <v>0.3160445362</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23">
         <v>15</v>
@@ -1380,15 +1383,15 @@
         <v>0.37820622349999999</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24">
         <v>23</v>
@@ -1418,18 +1421,18 @@
         <v>0.28345082659999998</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E25">
         <v>16</v>
@@ -1456,12 +1459,12 @@
         <v>0.34958613160000002</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
@@ -1494,18 +1497,18 @@
         <v>0.13594370710000001</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C27">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E27">
         <v>49</v>
@@ -1532,15 +1535,15 @@
         <v>0.15996502639999999</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D28">
         <v>27</v>
@@ -1570,18 +1573,18 @@
         <v>0.19978628970000001</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -1608,15 +1611,15 @@
         <v>0.22431699869999999</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D30">
         <v>29</v>
@@ -1646,18 +1649,18 @@
         <v>0.21992953679999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31">
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E31">
         <v>13</v>
@@ -1684,15 +1687,15 @@
         <v>0.2734302247</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D32">
         <v>31</v>
@@ -1722,18 +1725,18 @@
         <v>0.32801916650000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C33">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E33">
         <v>8</v>
@@ -1760,15 +1763,15 @@
         <v>0.36120855959999998</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D34">
         <v>33</v>
@@ -1798,18 +1801,18 @@
         <v>0.19577280920000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35">
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E35">
         <v>15</v>
@@ -1836,18 +1839,18 @@
         <v>0.25725838020000003</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E36">
         <v>86</v>
@@ -1874,15 +1877,15 @@
         <v>5.6027913899999997E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D37">
         <v>36</v>
@@ -1912,18 +1915,18 @@
         <v>0.3789065338</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C38">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E38">
         <v>18</v>
@@ -1950,18 +1953,18 @@
         <v>0.4534698674</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
         <v>32</v>
-      </c>
-      <c r="D39" t="s">
-        <v>34</v>
       </c>
       <c r="E39">
         <v>33</v>
@@ -1988,18 +1991,18 @@
         <v>0.18883525409999999</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E40">
         <v>40</v>
@@ -2026,18 +2029,18 @@
         <v>0.2176665434</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E41">
         <v>57</v>
@@ -2064,12 +2067,12 @@
         <v>0.28786746699999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
         <v>13</v>
@@ -2102,12 +2105,12 @@
         <v>5.65088386E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>90</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C43">
         <v>41</v>
@@ -2140,18 +2143,18 @@
         <v>6.7129100299999994E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C44">
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E44">
         <v>23</v>
@@ -2178,18 +2181,18 @@
         <v>7.8290485000000007E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E45">
         <v>17</v>
@@ -2216,18 +2219,18 @@
         <v>0.14592316750000001</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="s">
         <v>37</v>
-      </c>
-      <c r="D46" t="s">
-        <v>39</v>
       </c>
       <c r="E46">
         <v>22</v>
@@ -2254,15 +2257,15 @@
         <v>0.16627666620000001</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D47">
         <v>46</v>
@@ -2292,12 +2295,12 @@
         <v>0.1136555279</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C48">
         <v>46</v>
@@ -2330,18 +2333,18 @@
         <v>0.1216754887</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C49">
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E49">
         <v>20</v>
@@ -2368,18 +2371,18 @@
         <v>0.20311478559999999</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E50">
         <v>50</v>
@@ -2406,18 +2409,18 @@
         <v>0.28132635090000002</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E51">
         <v>42</v>
@@ -2444,18 +2447,18 @@
         <v>0.24834623010000001</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E52">
         <v>30</v>
@@ -2482,12 +2485,12 @@
         <v>0.19901227260000001</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C53" t="s">
         <v>13</v>
@@ -2520,18 +2523,18 @@
         <v>5.6027913899999997E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>90</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C54">
         <v>52</v>
       </c>
       <c r="D54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E54">
         <v>130</v>
@@ -2558,15 +2561,15 @@
         <v>0.11929406419999999</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D55">
         <v>54</v>
@@ -2596,18 +2599,18 @@
         <v>0.14696061939999999</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>90</v>
       </c>
       <c r="B56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C56">
         <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E56">
         <v>8</v>
@@ -2634,15 +2637,15 @@
         <v>0.17957796810000001</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>90</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D57">
         <v>56</v>
@@ -2672,18 +2675,18 @@
         <v>0.1912664791</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>90</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C58">
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E58">
         <v>7</v>
@@ -2710,15 +2713,15 @@
         <v>0.2201248052</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>90</v>
       </c>
       <c r="B59" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D59">
         <v>58</v>
@@ -2748,18 +2751,18 @@
         <v>0.18721204390000001</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>90</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C60">
         <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E60">
         <v>9</v>
@@ -2786,15 +2789,15 @@
         <v>0.22431083739999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D61">
         <v>60</v>
@@ -2824,18 +2827,18 @@
         <v>0.27295812060000002</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C62">
         <v>60</v>
       </c>
       <c r="D62" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E62">
         <v>7</v>
@@ -2862,15 +2865,15 @@
         <v>0.3020636666</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D63">
         <v>62</v>
@@ -2900,18 +2903,18 @@
         <v>0.28116929699999998</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C64">
         <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E64">
         <v>6</v>
@@ -2938,15 +2941,15 @@
         <v>0.3061263219</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D65">
         <v>64</v>
@@ -2976,18 +2979,18 @@
         <v>0.330529289</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>90</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C66">
         <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E66">
         <v>18</v>
@@ -3014,15 +3017,15 @@
         <v>0.4047703761</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>90</v>
       </c>
       <c r="B67" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D67">
         <v>66</v>
@@ -3052,18 +3055,18 @@
         <v>0.14696061939999999</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>90</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C68">
         <v>66</v>
       </c>
       <c r="D68" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E68">
         <v>18</v>
@@ -3090,15 +3093,15 @@
         <v>0.21974735749999999</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>90</v>
       </c>
       <c r="B69" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D69">
         <v>68</v>
@@ -3128,18 +3131,18 @@
         <v>0.2401741235</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C70">
         <v>68</v>
       </c>
       <c r="D70" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E70">
         <v>5</v>
@@ -3166,15 +3169,15 @@
         <v>0.2609080191</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>90</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C71" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D71">
         <v>70</v>
@@ -3204,18 +3207,18 @@
         <v>0.23199657439999999</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>90</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C72">
         <v>70</v>
       </c>
       <c r="D72" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E72">
         <v>6</v>
@@ -3242,12 +3245,12 @@
         <v>0.25686169380000001</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C73" t="s">
         <v>13</v>
@@ -3280,18 +3283,18 @@
         <v>8.0722394500000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C74">
         <v>72</v>
       </c>
       <c r="D74" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E74">
         <v>116</v>
@@ -3318,18 +3321,18 @@
         <v>0.13741361639999999</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D75" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E75">
         <v>29</v>
@@ -3356,18 +3359,18 @@
         <v>0.255787655</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" t="s">
         <v>54</v>
-      </c>
-      <c r="D76" t="s">
-        <v>56</v>
       </c>
       <c r="E76">
         <v>26</v>
@@ -3394,18 +3397,18 @@
         <v>0.24340221570000001</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>90</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C77" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D77" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E77">
         <v>47</v>
@@ -3432,12 +3435,12 @@
         <v>0.3303807674</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>90</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C78" t="s">
         <v>13</v>
@@ -3470,18 +3473,18 @@
         <v>8.0722394500000003E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C79">
         <v>77</v>
       </c>
       <c r="D79" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E79">
         <v>59</v>
@@ -3508,18 +3511,18 @@
         <v>0.1095103402</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C80" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D80" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E80">
         <v>27</v>
@@ -3546,18 +3549,18 @@
         <v>0.21954125990000001</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>90</v>
       </c>
       <c r="B81" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" t="s">
         <v>58</v>
-      </c>
-      <c r="D81" t="s">
-        <v>60</v>
       </c>
       <c r="E81">
         <v>30</v>
@@ -3584,18 +3587,18 @@
         <v>0.2319468391</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>90</v>
       </c>
       <c r="B82" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C82" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D82" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E82">
         <v>46</v>
@@ -3622,18 +3625,18 @@
         <v>0.29833162829999998</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>90</v>
       </c>
       <c r="B83" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C83" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D83" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E83">
         <v>62</v>
@@ -3660,18 +3663,18 @@
         <v>0.36494091709999998</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C84" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D84" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E84">
         <v>28</v>
@@ -3698,15 +3701,15 @@
         <v>0.22367451259999999</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C85" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D85">
         <v>84</v>
@@ -3736,18 +3739,18 @@
         <v>0.14112253359999999</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C86">
         <v>84</v>
       </c>
       <c r="D86" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E86">
         <v>27</v>
@@ -3774,12 +3777,12 @@
         <v>0.25224247910000003</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C87" t="s">
         <v>13</v>
@@ -3812,12 +3815,12 @@
         <v>8.1695614599999994E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C88">
         <v>86</v>
@@ -3850,18 +3853,18 @@
         <v>0.1099993108</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C89">
         <v>87</v>
       </c>
       <c r="D89" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E89">
         <v>58</v>
@@ -3888,18 +3891,18 @@
         <v>0.1383936345</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C90" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D90" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E90">
         <v>21</v>
@@ -3926,18 +3929,18 @@
         <v>0.22378688790000001</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C91" t="s">
+        <v>63</v>
+      </c>
+      <c r="D91" t="s">
         <v>65</v>
-      </c>
-      <c r="D91" t="s">
-        <v>67</v>
       </c>
       <c r="E91">
         <v>37</v>
@@ -3964,18 +3967,18 @@
         <v>0.28987078150000001</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C92" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D92" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E92">
         <v>27</v>
@@ -4002,12 +4005,12 @@
         <v>0.24851092960000001</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C93" t="s">
         <v>13</v>
@@ -4040,18 +4043,18 @@
         <v>6.5677055799999995E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>90</v>
       </c>
       <c r="B94" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C94">
         <v>92</v>
       </c>
       <c r="D94" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E94">
         <v>148</v>
@@ -4078,18 +4081,18 @@
         <v>0.13790362619999999</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C95" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D95" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E95">
         <v>29</v>
@@ -4116,18 +4119,18 @@
         <v>0.25472469599999997</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>90</v>
       </c>
       <c r="B96" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C96" t="s">
+        <v>67</v>
+      </c>
+      <c r="D96" t="s">
         <v>69</v>
-      </c>
-      <c r="D96" t="s">
-        <v>71</v>
       </c>
       <c r="E96">
         <v>37</v>
@@ -4154,18 +4157,18 @@
         <v>0.28746324029999998</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>90</v>
       </c>
       <c r="B97" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C97" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D97" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E97">
         <v>97</v>
@@ -4192,18 +4195,18 @@
         <v>0.18547880689999999</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>90</v>
       </c>
       <c r="B98" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C98" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D98" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E98">
         <v>45</v>
@@ -4230,15 +4233,15 @@
         <v>0.37009030059999998</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>90</v>
       </c>
       <c r="B99" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D99">
         <v>98</v>
@@ -4268,15 +4271,15 @@
         <v>0.2316333458</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>90</v>
       </c>
       <c r="B100" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C100" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D100">
         <v>99</v>
@@ -4306,12 +4309,12 @@
         <v>0.27791250010000002</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>90</v>
       </c>
       <c r="B101" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C101">
         <v>99</v>
@@ -4344,15 +4347,15 @@
         <v>0.33091493649999998</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>90</v>
       </c>
       <c r="B102" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C102" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D102" s="1">
         <v>101232740</v>
@@ -4382,15 +4385,15 @@
         <v>0.4006067988</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>90</v>
       </c>
       <c r="B103" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C103" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D103" s="1">
         <v>102232742</v>
@@ -4420,15 +4423,15 @@
         <v>0.25358431219999999</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C104" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D104" s="1">
         <v>103232743</v>
@@ -4458,15 +4461,15 @@
         <v>0.37597323329999999</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>90</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C105" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D105" s="1">
         <v>104232833</v>
@@ -4496,15 +4499,15 @@
         <v>0.25358431219999999</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>90</v>
       </c>
       <c r="B106" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C106" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D106" s="1">
         <v>105232744</v>
@@ -4534,15 +4537,15 @@
         <v>0.35319806269999998</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>90</v>
       </c>
       <c r="B107" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C107" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D107" s="1">
         <v>106232745</v>
@@ -4572,15 +4575,15 @@
         <v>0.21400088580000001</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>90</v>
       </c>
       <c r="B108" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C108" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D108" s="1">
         <v>107232746</v>
@@ -4610,12 +4613,12 @@
         <v>0.25472469599999997</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>90</v>
       </c>
       <c r="B109" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C109" t="s">
         <v>13</v>
@@ -4648,12 +4651,12 @@
         <v>1.9075819500000001E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>90</v>
       </c>
       <c r="B110" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C110" t="s">
         <v>13</v>
@@ -4686,12 +4689,12 @@
         <v>3.42407869E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>90</v>
       </c>
       <c r="B111" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C111" s="1">
         <v>1091153</v>
@@ -4724,12 +4727,12 @@
         <v>0.15814009039999999</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>90</v>
       </c>
       <c r="B112" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C112" s="1">
         <v>1091153</v>
@@ -4762,12 +4765,12 @@
         <v>0.27797634310000002</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>90</v>
       </c>
       <c r="B113" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C113" s="1">
         <v>1091153</v>
@@ -4800,12 +4803,12 @@
         <v>0.15814009039999999</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>90</v>
       </c>
       <c r="B114" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C114" s="1">
         <v>1091153</v>
@@ -4838,12 +4841,12 @@
         <v>6.5193272199999999E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>90</v>
       </c>
       <c r="B115" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C115" s="1">
         <v>1131152</v>
@@ -4876,12 +4879,12 @@
         <v>0.23929802680000001</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>90</v>
       </c>
       <c r="B116" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C116" s="1">
         <v>1131152</v>
@@ -4914,12 +4917,12 @@
         <v>0.2599248348</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>90</v>
       </c>
       <c r="B117" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C117" s="1">
         <v>1131152</v>
@@ -4952,12 +4955,12 @@
         <v>0.3136300863</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>90</v>
       </c>
       <c r="B118" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C118" s="1">
         <v>1131152</v>
@@ -4990,12 +4993,12 @@
         <v>0.23929802680000001</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>90</v>
       </c>
       <c r="B119" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C119" s="1">
         <v>1131152</v>
@@ -5028,12 +5031,12 @@
         <v>0.1245407159</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>90</v>
       </c>
       <c r="B120" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C120" s="1">
         <v>1131152</v>
@@ -5066,12 +5069,12 @@
         <v>0.14894402500000001</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>90</v>
       </c>
       <c r="B121" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C121" s="1">
         <v>1091153</v>
@@ -5104,12 +5107,12 @@
         <v>0.1129680862</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>90</v>
       </c>
       <c r="B122" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C122" t="s">
         <v>13</v>
@@ -5142,12 +5145,12 @@
         <v>0.26692134820000002</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>90</v>
       </c>
       <c r="B123" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C123" s="1">
         <v>1210047</v>
@@ -5186,23 +5189,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_lisam_Description xmlns="1dc47e02-2fe9-4d00-8f29-253b519e6342" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100CBF7FAF46625674D856C12A9888664B2" ma:contentTypeVersion="5" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="3b6c61bdc3075b731ac400c18a8bcfe0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1dc47e02-2fe9-4d00-8f29-253b519e6342" xmlns:ns3="b90ed1ef-56ea-4a5f-889a-5350cb6cd4db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea2049e3d60e769c42ad32b82175f215" ns2:_="" ns3:_="">
     <xsd:import namespace="1dc47e02-2fe9-4d00-8f29-253b519e6342"/>
@@ -5361,25 +5347,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75006BDD-3E20-48FF-9486-610A487F54ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1dc47e02-2fe9-4d00-8f29-253b519e6342"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_lisam_Description xmlns="1dc47e02-2fe9-4d00-8f29-253b519e6342" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AE805CF-F14E-43F1-BD2F-AF33A7F9DB90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF0980-F77A-40DF-A94C-BC222A8DDBD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5396,4 +5381,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75006BDD-3E20-48FF-9486-610A487F54ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1dc47e02-2fe9-4d00-8f29-253b519e6342"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AE805CF-F14E-43F1-BD2F-AF33A7F9DB90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>